<commit_message>
fix #333 EU-NIS2 notice report definitions
Co-authored-by: Arthit Suriyawongkul <arthit@gmail.com>
</commit_message>
<xml_diff>
--- a/code/vocab_csv/eu-nis2.xlsx
+++ b/code/vocab_csv/eu-nis2.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="74">
   <si>
     <t>Term</t>
   </si>
@@ -90,7 +90,16 @@
     <t>Early Warning Report</t>
   </si>
   <si>
-    <t>within 24 hours of detection containing cause of the incident and whether it was unlawful or malicious and whether there is cross-border impact</t>
+    <t>Report sent within 24 hours of detection containing cause of the incident and whether it was unlawful or malicious and whether there is cross-border impact</t>
+  </si>
+  <si>
+    <t>NIS2 Article 23 (4)(a)</t>
+  </si>
+  <si>
+    <t>modified</t>
+  </si>
+  <si>
+    <t>Harshvardhan J. Pandit, Georg P. Krog, Arthit Suriyawongkul</t>
   </si>
   <si>
     <t>IncidentAssessmentReport</t>
@@ -99,7 +108,10 @@
     <t>Incident Assessment Report</t>
   </si>
   <si>
-    <t>within 72 hours of detection, which contains updates on the earlier information as well as initial assessment of severity and impact of the incident as well as any 'indicators of compromise'</t>
+    <t>Report sent within 72 hours of detection containing updates on the earlier information as well as initial assessment of severity and impact of the incident as well as any 'indicators of compromise'</t>
+  </si>
+  <si>
+    <t>NIS2 Article 23 (4)(b)</t>
   </si>
   <si>
     <t>IntermediateReport</t>
@@ -108,7 +120,10 @@
     <t>Intermediate Report</t>
   </si>
   <si>
-    <t>upon request - which provides updates, if any, to previous information</t>
+    <t>Report sent upon request which provides updates, if any, to previous information</t>
+  </si>
+  <si>
+    <t>NIS2 Article 23 (4)(c)</t>
   </si>
   <si>
     <t>ProgressReport</t>
@@ -117,7 +132,10 @@
     <t>Progress Report</t>
   </si>
   <si>
-    <t>within 1 month of detection if the incident handling has not been completed by then, with updates to previous information</t>
+    <t>Report sent within 1 month of detection if the incident handling has not been completed by then, with updates to previous information</t>
+  </si>
+  <si>
+    <t>NIS2 Article 23 (4)(e)</t>
   </si>
   <si>
     <t>FinalReport</t>
@@ -126,7 +144,10 @@
     <t>Final Report</t>
   </si>
   <si>
-    <t>within 1 month of incident handling i.e. completing the incident recovery and containing the applied/ongoing measures, 'detailed description' - not sure what this means, and threat type / root cause - which is covered with threat and vulnerability concepts</t>
+    <t>Report sent within 1 month of incident handling i.e. completing the incident recovery and containing the applied/ongoing measures, and containing a 'detailed description' of the incident including its severityand impact, threat type and root cause that are likely to have triggered the incident, applied and ongoing measures, and - if applicable - cross-border impacts</t>
+  </si>
+  <si>
+    <t>NIS2 Article 23 (4)(d)</t>
   </si>
   <si>
     <t>InitialFeedbackOnIncident</t>
@@ -805,245 +826,155 @@
       <c r="C3" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="11"/>
       <c r="E3" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
       <c r="J3" s="9" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="K3" s="12">
         <v>45431.0</v>
       </c>
-      <c r="L3" s="11"/>
+      <c r="L3" s="14">
+        <v>45874.0</v>
+      </c>
       <c r="M3" s="9" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="N3" s="9" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="O3" s="13"/>
-      <c r="P3" s="11"/>
-      <c r="Q3" s="11"/>
-      <c r="R3" s="11"/>
-      <c r="S3" s="11"/>
-      <c r="T3" s="11"/>
-      <c r="U3" s="11"/>
-      <c r="V3" s="11"/>
-      <c r="W3" s="11"/>
-      <c r="X3" s="11"/>
-      <c r="Y3" s="11"/>
-      <c r="Z3" s="11"/>
-      <c r="AA3" s="11"/>
-      <c r="AB3" s="11"/>
-      <c r="AC3" s="11"/>
-      <c r="AD3" s="11"/>
     </row>
     <row r="4">
       <c r="A4" s="9" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="11"/>
+        <v>31</v>
+      </c>
       <c r="E4" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
       <c r="J4" s="9" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="K4" s="12">
         <v>45431.0</v>
       </c>
-      <c r="L4" s="11"/>
+      <c r="L4" s="14">
+        <v>45874.0</v>
+      </c>
       <c r="M4" s="9" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="O4" s="13"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="11"/>
-      <c r="S4" s="11"/>
-      <c r="T4" s="11"/>
-      <c r="U4" s="11"/>
-      <c r="V4" s="11"/>
-      <c r="W4" s="11"/>
-      <c r="X4" s="11"/>
-      <c r="Y4" s="11"/>
-      <c r="Z4" s="11"/>
-      <c r="AA4" s="11"/>
-      <c r="AB4" s="11"/>
-      <c r="AC4" s="11"/>
-      <c r="AD4" s="11"/>
     </row>
     <row r="5">
       <c r="A5" s="9" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="11"/>
+        <v>35</v>
+      </c>
       <c r="E5" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
       <c r="J5" s="9" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="K5" s="12">
         <v>45431.0</v>
       </c>
-      <c r="L5" s="11"/>
+      <c r="L5" s="14">
+        <v>45874.0</v>
+      </c>
       <c r="M5" s="9" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="N5" s="9" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="O5" s="13"/>
-      <c r="P5" s="11"/>
-      <c r="Q5" s="11"/>
-      <c r="R5" s="11"/>
-      <c r="S5" s="11"/>
-      <c r="T5" s="11"/>
-      <c r="U5" s="11"/>
-      <c r="V5" s="11"/>
-      <c r="W5" s="11"/>
-      <c r="X5" s="11"/>
-      <c r="Y5" s="11"/>
-      <c r="Z5" s="11"/>
-      <c r="AA5" s="11"/>
-      <c r="AB5" s="11"/>
-      <c r="AC5" s="11"/>
-      <c r="AD5" s="11"/>
     </row>
     <row r="6">
       <c r="A6" s="9" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" s="11"/>
+        <v>39</v>
+      </c>
       <c r="E6" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
       <c r="J6" s="9" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="K6" s="12">
         <v>45431.0</v>
       </c>
-      <c r="L6" s="11"/>
+      <c r="L6" s="14">
+        <v>45874.0</v>
+      </c>
       <c r="M6" s="9" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="N6" s="9" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="O6" s="13"/>
-      <c r="P6" s="11"/>
-      <c r="Q6" s="11"/>
-      <c r="R6" s="11"/>
-      <c r="S6" s="11"/>
-      <c r="T6" s="11"/>
-      <c r="U6" s="11"/>
-      <c r="V6" s="11"/>
-      <c r="W6" s="11"/>
-      <c r="X6" s="11"/>
-      <c r="Y6" s="11"/>
-      <c r="Z6" s="11"/>
-      <c r="AA6" s="11"/>
-      <c r="AB6" s="11"/>
-      <c r="AC6" s="11"/>
-      <c r="AD6" s="11"/>
     </row>
     <row r="7">
       <c r="A7" s="9" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" s="11"/>
+        <v>43</v>
+      </c>
       <c r="E7" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
       <c r="J7" s="9" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="K7" s="12">
         <v>45431.0</v>
       </c>
-      <c r="L7" s="11"/>
+      <c r="L7" s="14">
+        <v>45874.0</v>
+      </c>
       <c r="M7" s="9" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="N7" s="9" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="O7" s="13"/>
-      <c r="P7" s="11"/>
-      <c r="Q7" s="11"/>
-      <c r="R7" s="11"/>
-      <c r="S7" s="11"/>
-      <c r="T7" s="11"/>
-      <c r="U7" s="11"/>
-      <c r="V7" s="11"/>
-      <c r="W7" s="11"/>
-      <c r="X7" s="11"/>
-      <c r="Y7" s="11"/>
-      <c r="Z7" s="11"/>
-      <c r="AA7" s="11"/>
-      <c r="AB7" s="11"/>
-      <c r="AC7" s="11"/>
-      <c r="AD7" s="11"/>
     </row>
     <row r="8">
       <c r="A8" s="9" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D8" s="11"/>
       <c r="E8" s="9" t="s">
@@ -1085,13 +1016,13 @@
     </row>
     <row r="9">
       <c r="A9" s="9" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="9" t="s">
@@ -1136,7 +1067,7 @@
     </row>
     <row r="11">
       <c r="A11" s="15" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="K11" s="14"/>
     </row>
@@ -1145,19 +1076,19 @@
     </row>
     <row r="13">
       <c r="A13" s="9" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="K13" s="14"/>
     </row>
     <row r="14">
       <c r="A14" s="9" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="K14" s="14"/>
     </row>
     <row r="15">
       <c r="A15" s="9" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1217,13 +1148,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
@@ -4366,7 +4297,7 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C2" s="10"/>
       <c r="K2" s="12"/>
@@ -4374,17 +4305,17 @@
     </row>
     <row r="3">
       <c r="A3" s="9" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="9" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="F3" s="11"/>
       <c r="G3" s="11"/>
@@ -4399,7 +4330,7 @@
         <v>21</v>
       </c>
       <c r="N3" s="9" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="O3" s="13"/>
       <c r="P3" s="11"/>
@@ -4420,19 +4351,19 @@
     </row>
     <row r="4">
       <c r="A4" s="9" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
@@ -4447,7 +4378,7 @@
         <v>21</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="O4" s="13"/>
       <c r="P4" s="11"/>
@@ -4468,19 +4399,19 @@
     </row>
     <row r="5">
       <c r="A5" s="9" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="B5" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="9" t="s">
         <v>62</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>55</v>
       </c>
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
@@ -4495,7 +4426,7 @@
         <v>21</v>
       </c>
       <c r="N5" s="9" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="O5" s="13"/>
       <c r="P5" s="11"/>
@@ -4516,19 +4447,19 @@
     </row>
     <row r="6">
       <c r="A6" s="9" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
@@ -4543,7 +4474,7 @@
         <v>21</v>
       </c>
       <c r="N6" s="9" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="O6" s="13"/>
       <c r="P6" s="11"/>

</xml_diff>

<commit_message>
Update EU-NIS2 source (#348)
* Update EU-NIS2 source

Update source to be more specific for
- SignificantIncidentNotice
- InitialFeedbackOnIncident
- RiskMitigationAdvice

Follow up of #333

Signed-off-by: Arthit Suriyawongkul <arthit@gmail.com>

* Use "NIS2"

Signed-off-by: Arthit Suriyawongkul <arthit@gmail.com>

---------

Signed-off-by: Arthit Suriyawongkul <arthit@gmail.com>
</commit_message>
<xml_diff>
--- a/code/vocab_csv/eu-nis2.xlsx
+++ b/code/vocab_csv/eu-nis2.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="75">
   <si>
     <t>Term</t>
   </si>
@@ -75,7 +75,7 @@
     <t>sc</t>
   </si>
   <si>
-    <t>NIS2 Directive</t>
+    <t>NIS2 Article 23(3)</t>
   </si>
   <si>
     <t>accepted</t>
@@ -93,7 +93,7 @@
     <t>Report sent within 24 hours of detection containing cause of the incident and whether it was unlawful or malicious and whether there is cross-border impact</t>
   </si>
   <si>
-    <t>NIS2 Article 23 (4)(a)</t>
+    <t>NIS2 Article 23(4)(a)</t>
   </si>
   <si>
     <t>modified</t>
@@ -111,7 +111,7 @@
     <t>Report sent within 72 hours of detection containing updates on the earlier information as well as initial assessment of severity and impact of the incident as well as any 'indicators of compromise'</t>
   </si>
   <si>
-    <t>NIS2 Article 23 (4)(b)</t>
+    <t>NIS2 Article 23(4)(b)</t>
   </si>
   <si>
     <t>IntermediateReport</t>
@@ -123,7 +123,7 @@
     <t>Report sent upon request which provides updates, if any, to previous information</t>
   </si>
   <si>
-    <t>NIS2 Article 23 (4)(c)</t>
+    <t>NIS2 Article 23(4)(c)</t>
   </si>
   <si>
     <t>ProgressReport</t>
@@ -135,7 +135,7 @@
     <t>Report sent within 1 month of detection if the incident handling has not been completed by then, with updates to previous information</t>
   </si>
   <si>
-    <t>NIS2 Article 23 (4)(e)</t>
+    <t>NIS2 Article 23(4)(e)</t>
   </si>
   <si>
     <t>FinalReport</t>
@@ -144,10 +144,10 @@
     <t>Final Report</t>
   </si>
   <si>
-    <t>Report sent within 1 month of incident handling i.e. completing the incident recovery and containing the applied/ongoing measures, and containing a 'detailed description' of the incident including its severityand impact, threat type and root cause that are likely to have triggered the incident, applied and ongoing measures, and - if applicable - cross-border impacts</t>
-  </si>
-  <si>
-    <t>NIS2 Article 23 (4)(d)</t>
+    <t>Report sent within 1 month of incident handling i.e. completing the incident recovery and containing the applied/ongoing measures, and containing a 'detailed description' of the incident including its severity and impact, threat type and root cause that are likely to have triggered the incident, applied and ongoing measures, and - if applicable - cross-border impacts</t>
+  </si>
+  <si>
+    <t>NIS2 Article 23(4)(d)</t>
   </si>
   <si>
     <t>InitialFeedbackOnIncident</t>
@@ -157,6 +157,9 @@
   </si>
   <si>
     <t>Notification from authority to organisation (upon request, within 24 hours or early warning) containing "initial feedback" and guidelines on measures that can be taken in response to a breach</t>
+  </si>
+  <si>
+    <t>NIS2 Article 23(5)</t>
   </si>
   <si>
     <t>RiskMitigationAdvice</t>
@@ -717,6 +720,7 @@
     <col customWidth="1" min="1" max="1" width="32.13"/>
     <col customWidth="1" min="2" max="2" width="20.88"/>
     <col customWidth="1" min="3" max="3" width="38.5"/>
+    <col customWidth="1" min="10" max="10" width="28.13"/>
   </cols>
   <sheetData>
     <row r="1" ht="28.5" customHeight="1">
@@ -985,7 +989,7 @@
       <c r="H8" s="11"/>
       <c r="I8" s="11"/>
       <c r="J8" s="9" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="K8" s="12">
         <v>45431.0</v>
@@ -1016,13 +1020,13 @@
     </row>
     <row r="9">
       <c r="A9" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="9" t="s">
@@ -1033,7 +1037,7 @@
       <c r="H9" s="11"/>
       <c r="I9" s="11"/>
       <c r="J9" s="9" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="K9" s="12">
         <v>45431.0</v>
@@ -1067,7 +1071,7 @@
     </row>
     <row r="11">
       <c r="A11" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K11" s="14"/>
     </row>
@@ -1076,19 +1080,19 @@
     </row>
     <row r="13">
       <c r="A13" s="9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K13" s="14"/>
     </row>
     <row r="14">
       <c r="A14" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K14" s="14"/>
     </row>
     <row r="15">
       <c r="A15" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1148,13 +1152,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
@@ -4297,7 +4301,7 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C2" s="10"/>
       <c r="K2" s="12"/>
@@ -4305,17 +4309,17 @@
     </row>
     <row r="3">
       <c r="A3" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F3" s="11"/>
       <c r="G3" s="11"/>
@@ -4330,7 +4334,7 @@
         <v>21</v>
       </c>
       <c r="N3" s="9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="O3" s="13"/>
       <c r="P3" s="11"/>
@@ -4351,19 +4355,19 @@
     </row>
     <row r="4">
       <c r="A4" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
@@ -4378,7 +4382,7 @@
         <v>21</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="O4" s="13"/>
       <c r="P4" s="11"/>
@@ -4399,19 +4403,19 @@
     </row>
     <row r="5">
       <c r="A5" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>67</v>
-      </c>
       <c r="E5" s="9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
@@ -4426,7 +4430,7 @@
         <v>21</v>
       </c>
       <c r="N5" s="9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="O5" s="13"/>
       <c r="P5" s="11"/>
@@ -4447,19 +4451,19 @@
     </row>
     <row r="6">
       <c r="A6" s="9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
@@ -4474,7 +4478,7 @@
         <v>21</v>
       </c>
       <c r="N6" s="9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="O6" s="13"/>
       <c r="P6" s="11"/>

</xml_diff>